<commit_message>
adding RDW file intergration to repo
</commit_message>
<xml_diff>
--- a/Doc/iApply_Integration.xlsx
+++ b/Doc/iApply_Integration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ven-talent-axwar\Documents\ACWAR\iApply_Integration\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D939B91B-7695-4A70-84D3-771EAA942D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCDD196-FA7E-489A-928E-D2D2814C1250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89D5BFD2-F8FE-4C40-A489-08526D236723}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="197">
   <si>
     <t>iApply Form Name</t>
   </si>
@@ -639,6 +639,21 @@
   </si>
   <si>
     <t>ODO</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -1373,13 +1388,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7847A0BE-24C9-4B51-84A9-78CA288F75CC}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1549,7 +1564,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" hidden="1">
+    <row r="4" spans="1:16" s="1" customFormat="1">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -1599,7 +1614,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" hidden="1">
+    <row r="5" spans="1:16" s="1" customFormat="1">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -1691,7 +1706,7 @@
       <c r="O6" s="20"/>
       <c r="P6" s="39"/>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" hidden="1">
+    <row r="7" spans="1:16" s="1" customFormat="1">
       <c r="A7" s="20">
         <v>6</v>
       </c>
@@ -1741,7 +1756,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" hidden="1">
+    <row r="8" spans="1:16" s="1" customFormat="1">
       <c r="A8" s="20">
         <v>7</v>
       </c>
@@ -1841,7 +1856,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" hidden="1">
+    <row r="10" spans="1:16" s="1" customFormat="1">
       <c r="A10" s="20">
         <v>9</v>
       </c>
@@ -1891,7 +1906,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" hidden="1">
+    <row r="11" spans="1:16" s="1" customFormat="1">
       <c r="A11" s="20">
         <v>10</v>
       </c>
@@ -1941,7 +1956,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+    <row r="12" spans="1:16" s="2" customFormat="1" ht="25.5" customHeight="1">
       <c r="A12" s="20">
         <v>11</v>
       </c>
@@ -1991,7 +2006,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+    <row r="13" spans="1:16" s="2" customFormat="1" ht="25.5" customHeight="1">
       <c r="A13" s="20">
         <v>12</v>
       </c>
@@ -2002,28 +2017,28 @@
         <v>59</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>10</v>
+        <v>116</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="L13" s="20" t="s">
         <v>10</v>
@@ -2041,7 +2056,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" hidden="1">
+    <row r="14" spans="1:16" s="1" customFormat="1">
       <c r="A14" s="20">
         <v>13</v>
       </c>
@@ -2091,7 +2106,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="52" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+    <row r="15" spans="1:16" s="52" customFormat="1" ht="25.5" customHeight="1">
       <c r="A15" s="20">
         <v>14</v>
       </c>
@@ -2191,7 +2206,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="18" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+    <row r="17" spans="1:16" s="18" customFormat="1" ht="25.5" customHeight="1">
       <c r="A17" s="20">
         <v>16</v>
       </c>
@@ -2241,7 +2256,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="18" spans="1:16" s="18" customFormat="1">
       <c r="A18" s="20">
         <v>17</v>
       </c>
@@ -2291,7 +2306,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="19" spans="1:16" s="18" customFormat="1">
       <c r="A19" s="20">
         <v>18</v>
       </c>
@@ -2391,7 +2406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="18" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="21" spans="1:16" s="18" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="20">
         <v>20</v>
       </c>
@@ -2439,7 +2454,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="22" spans="1:16" s="18" customFormat="1">
       <c r="A22" s="20">
         <v>21</v>
       </c>
@@ -2487,7 +2502,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="23" spans="1:16" s="18" customFormat="1">
       <c r="A23" s="20">
         <v>22</v>
       </c>
@@ -2535,7 +2550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="24" spans="1:16" s="18" customFormat="1">
       <c r="A24" s="20">
         <v>23</v>
       </c>
@@ -2583,7 +2598,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="25" spans="1:16" s="18" customFormat="1">
       <c r="A25" s="20">
         <v>24</v>
       </c>
@@ -2681,7 +2696,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="27" spans="1:16" s="18" customFormat="1">
       <c r="A27" s="20">
         <v>26</v>
       </c>
@@ -2729,7 +2744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="28" spans="1:16" s="18" customFormat="1">
       <c r="A28" s="20">
         <v>27</v>
       </c>
@@ -2777,7 +2792,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="29" spans="1:16" s="18" customFormat="1">
       <c r="A29" s="20">
         <v>28</v>
       </c>
@@ -2825,7 +2840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="30" spans="1:16" s="18" customFormat="1">
       <c r="A30" s="20">
         <v>29</v>
       </c>
@@ -2873,7 +2888,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="18" customFormat="1" hidden="1">
+    <row r="31" spans="1:16" s="18" customFormat="1">
       <c r="A31" s="20">
         <v>30</v>
       </c>
@@ -2971,7 +2986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+    <row r="33" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1">
       <c r="A33" s="20">
         <v>32</v>
       </c>
@@ -3019,7 +3034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1">
+    <row r="34" spans="1:16">
       <c r="A34" s="20">
         <v>33</v>
       </c>
@@ -3067,7 +3082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1">
+    <row r="35" spans="1:16">
       <c r="A35" s="20">
         <v>34</v>
       </c>
@@ -3115,7 +3130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1">
+    <row r="36" spans="1:16">
       <c r="A36" s="20">
         <v>35</v>
       </c>
@@ -3163,7 +3178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1">
+    <row r="37" spans="1:16">
       <c r="A37" s="20">
         <v>36</v>
       </c>
@@ -3259,7 +3274,7 @@
       </c>
       <c r="P38" s="47"/>
     </row>
-    <row r="39" spans="1:16" hidden="1">
+    <row r="39" spans="1:16">
       <c r="A39" s="20">
         <v>38</v>
       </c>
@@ -3307,7 +3322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1">
+    <row r="40" spans="1:16">
       <c r="A40" s="20">
         <v>39</v>
       </c>
@@ -3392,18 +3407,51 @@
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="3:4">
+    <row r="49" spans="3:5">
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
+    <row r="56" spans="3:5">
+      <c r="D56" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5">
+      <c r="D57" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5">
+      <c r="D58" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E58">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5">
+      <c r="D59" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E59">
+        <f>28*4</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5">
+      <c r="E60">
+        <f>E59+E58+E57+E56</f>
+        <v>1307</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:P40" xr:uid="{7238BF90-C5A5-456F-9783-350906B6602C}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="COMPLETE"/>
-        <filter val="NOT REQUIRED"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P38">
       <sortCondition ref="A1"/>
     </sortState>
@@ -3419,10 +3467,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20553A5C-2519-4299-A1F7-E6E69CB2C0B9}">
-  <dimension ref="A1:XDD34"/>
+  <dimension ref="A1:XDD55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4078,6 +4126,64 @@
       </c>
       <c r="F34" s="17" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="E45">
+        <f>10.4*4</f>
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6">
+      <c r="E49" t="s">
+        <v>192</v>
+      </c>
+      <c r="F49">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6">
+      <c r="E50" t="s">
+        <v>193</v>
+      </c>
+      <c r="F50">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6">
+      <c r="E51" t="s">
+        <v>194</v>
+      </c>
+      <c r="F51">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" spans="5:6">
+      <c r="E52" t="s">
+        <v>195</v>
+      </c>
+      <c r="F52">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="5:6">
+      <c r="E53" t="s">
+        <v>196</v>
+      </c>
+      <c r="F53">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="5:6">
+      <c r="F54">
+        <f>F53+F52+F51+F50+F49</f>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="55" spans="5:6">
+      <c r="F55">
+        <f>4400-1310</f>
+        <v>3090</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding iApply form RDW into repo
</commit_message>
<xml_diff>
--- a/Doc/iApply_Integration.xlsx
+++ b/Doc/iApply_Integration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ven-talent-axwar\Documents\ACWAR\iApply_Integration\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCDD196-FA7E-489A-928E-D2D2814C1250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7431F3FA-86E1-4A5C-A265-C583885E9118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89D5BFD2-F8FE-4C40-A489-08526D236723}"/>
   </bookViews>
@@ -1394,7 +1394,7 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2043,8 +2043,8 @@
       <c r="L13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="20" t="s">
-        <v>10</v>
+      <c r="M13" s="45" t="s">
+        <v>106</v>
       </c>
       <c r="N13" s="59">
         <v>44666</v>

</xml_diff>

<commit_message>
adding files to RDW form to repo
</commit_message>
<xml_diff>
--- a/Doc/iApply_Integration.xlsx
+++ b/Doc/iApply_Integration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ven-talent-axwar\Documents\ACWAR\iApply_Integration\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7431F3FA-86E1-4A5C-A265-C583885E9118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17FBE29-51D3-4CC0-B183-10DC154BBF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89D5BFD2-F8FE-4C40-A489-08526D236723}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89D5BFD2-F8FE-4C40-A489-08526D236723}"/>
   </bookViews>
   <sheets>
     <sheet name="iApply_Integration_Overall_Stat" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="198">
   <si>
     <t>iApply Form Name</t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>LIVE - 01 Jul 2022 [1:12 PM]</t>
   </si>
 </sst>
 </file>
@@ -1391,7 +1394,7 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -2041,7 +2044,7 @@
         <v>69</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M13" s="45" t="s">
         <v>106</v>
@@ -2049,8 +2052,8 @@
       <c r="N13" s="59">
         <v>44666</v>
       </c>
-      <c r="O13" s="20" t="s">
-        <v>10</v>
+      <c r="O13" s="31" t="s">
+        <v>197</v>
       </c>
       <c r="P13" s="39" t="s">
         <v>163</v>
@@ -3407,47 +3410,14 @@
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="3:5">
+    <row r="49" spans="3:4">
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="56" spans="3:5">
-      <c r="D56" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E56">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="57" spans="3:5">
-      <c r="D57" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="E57">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="58" spans="3:5">
-      <c r="D58" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E58">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="3:5">
-      <c r="D59" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="E59">
-        <f>28*4</f>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5">
-      <c r="E60">
-        <f>E59+E58+E57+E56</f>
-        <v>1307</v>
+    <row r="52" spans="3:4">
+      <c r="C52" s="3">
+        <f>631+137+137+137</f>
+        <v>1042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding customer complaints form related sql files into repo
</commit_message>
<xml_diff>
--- a/Doc/iApply_Integration.xlsx
+++ b/Doc/iApply_Integration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ven-talent-axwar\Documents\ACWAR\iApply_Integration\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17FBE29-51D3-4CC0-B183-10DC154BBF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CED0D4-41ED-4F35-9953-DA48F430EFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89D5BFD2-F8FE-4C40-A489-08526D236723}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="43200" windowHeight="17235" xr2:uid="{89D5BFD2-F8FE-4C40-A489-08526D236723}"/>
   </bookViews>
   <sheets>
     <sheet name="iApply_Integration_Overall_Stat" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="201">
   <si>
     <t>iApply Form Name</t>
   </si>
@@ -657,6 +657,15 @@
   </si>
   <si>
     <t>LIVE - 01 Jul 2022 [1:12 PM]</t>
+  </si>
+  <si>
+    <t>Consumer complaints</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>Work in Progress</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1406,7 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3370,6 +3379,56 @@
         <v>10</v>
       </c>
       <c r="P40" s="47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="20">
+        <v>39</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="E41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="F41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="H41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="I41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="J41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="K41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="L41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="M41" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="N41" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="O41" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="P41" s="47" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>